<commit_message>
GPS tracking completed, need to enhance and add a few features to consider the whole story as completed
</commit_message>
<xml_diff>
--- a/CourseAdmin/GPS Setup Research (Final++).xlsx
+++ b/CourseAdmin/GPS Setup Research (Final++).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7992"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -210,12 +210,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,41 +510,41 @@
     <col min="17" max="16384" width="14.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:16" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -560,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="e">
-        <f t="shared" ref="D2:D11" si="0">DEGREES(ATAN2(ABS(RADIANS(B$2)-RADIANS(B2)),LN((TAN((RADIANS(A2)/2)+(PI()/4)))/(TAN((RADIANS(A$2)/2)+(PI()/4))))))</f>
+        <f>DEGREES(ATAN2(ABS(RADIANS(B$2)-RADIANS(B2)),LN((TAN((RADIANS(A2)/2)+(PI()/4)))/(TAN((RADIANS(A$2)/2)+(PI()/4))))))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E2" s="2" t="e">
@@ -586,7 +586,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M2" s="2" t="e">
-        <f t="shared" ref="M2:M11" si="1">I2/C2</f>
+        <f t="shared" ref="M2:M11" si="0">I2/C2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P2" s="2" t="e">
@@ -602,15 +602,15 @@
         <v>-73.641301999999996</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C11" si="2">6372.795477598*ACOS(SIN(RADIANS(A$2))*SIN(RADIANS(A3))+COS(RADIANS(A$2))*COS(RADIANS(A3))*COS(RADIANS(B$2-B3)))</f>
+        <f t="shared" ref="C3:C11" si="1">6372.795477598*ACOS(SIN(RADIANS(A$2))*SIN(RADIANS(A3))+COS(RADIANS(A$2))*COS(RADIANS(A3))*COS(RADIANS(B$2-B3)))</f>
         <v>2.1263867549245898E-2</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D2:D11" si="2">DEGREES(ATAN2(ABS(RADIANS(B$2)-RADIANS(B3)),LN((TAN((RADIANS(A3)/2)+(PI()/4)))/(TAN((RADIANS(A$2)/2)+(PI()/4))))))</f>
         <v>23.097935620873553</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E44" si="3">ABS(IF(B$2&gt;B3,D3+270,D3-90))</f>
+        <f t="shared" ref="E3:E11" si="3">ABS(IF(B$2&gt;B3,D3+270,D3-90))</f>
         <v>293.09793562087356</v>
       </c>
       <c r="G3" s="3">
@@ -632,7 +632,7 @@
         <v>289.44003482817618</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2543.4351961940174</v>
       </c>
       <c r="P3" s="2">
@@ -648,11 +648,11 @@
         <v>-73.641557000000006</v>
       </c>
       <c r="C4" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2393936303512639E-2</v>
+      </c>
+      <c r="D4" s="2">
         <f t="shared" si="2"/>
-        <v>4.2393936303512639E-2</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" si="0"/>
         <v>21.549765375734275</v>
       </c>
       <c r="E4" s="2">
@@ -678,7 +678,7 @@
         <v>290.19980662143411</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2664.2227644414475</v>
       </c>
       <c r="P4" s="2">
@@ -694,11 +694,11 @@
         <v>-73.641835</v>
       </c>
       <c r="C5" s="2">
+        <f t="shared" si="1"/>
+        <v>6.5729725610208664E-2</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" si="2"/>
-        <v>6.5729725610208664E-2</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="0"/>
         <v>21.647441348373139</v>
       </c>
       <c r="E5" s="2">
@@ -724,7 +724,7 @@
         <v>291.61477894278624</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2601.9629958459486</v>
       </c>
       <c r="P5" s="2">
@@ -740,11 +740,11 @@
         <v>-73.642106999999996</v>
       </c>
       <c r="C6" s="2">
+        <f t="shared" si="1"/>
+        <v>8.9135735039067091E-2</v>
+      </c>
+      <c r="D6" s="2">
         <f t="shared" si="2"/>
-        <v>8.9135735039067091E-2</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" si="0"/>
         <v>22.602253272767435</v>
       </c>
       <c r="E6" s="2">
@@ -770,7 +770,7 @@
         <v>291.89367314172841</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2587.4460892809157</v>
       </c>
       <c r="P6" s="2">
@@ -786,11 +786,11 @@
         <v>-73.642390000000006</v>
       </c>
       <c r="C7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11312870426258187</v>
+      </c>
+      <c r="D7" s="2">
         <f t="shared" si="2"/>
-        <v>0.11312870426258187</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="0"/>
         <v>22.730115923497472</v>
       </c>
       <c r="E7" s="2">
@@ -816,7 +816,7 @@
         <v>292.23273719388948</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2616.5486346646599</v>
       </c>
       <c r="P7" s="2">
@@ -832,11 +832,11 @@
         <v>-73.642685</v>
       </c>
       <c r="C8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13819977311359324</v>
+      </c>
+      <c r="D8" s="2">
         <f t="shared" si="2"/>
-        <v>0.13819977311359324</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
         <v>22.875451249430519</v>
       </c>
       <c r="E8" s="2">
@@ -862,7 +862,7 @@
         <v>292.27589784825898</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2596.0657377415732</v>
       </c>
       <c r="P8" s="2">
@@ -878,11 +878,11 @@
         <v>-73.642951999999994</v>
       </c>
       <c r="C9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16005954685925355</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="2"/>
-        <v>0.16005954685925355</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="0"/>
         <v>22.254632699817247</v>
       </c>
       <c r="E9" s="2">
@@ -908,7 +908,7 @@
         <v>291.59796327698291</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2613.866167921848</v>
       </c>
       <c r="P9" s="2">
@@ -924,11 +924,11 @@
         <v>-73.643197000000001</v>
       </c>
       <c r="C10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1813590244296909</v>
+      </c>
+      <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>0.1813590244296909</v>
-      </c>
-      <c r="D10" s="2">
-        <f t="shared" si="0"/>
         <v>22.767216443991625</v>
       </c>
       <c r="E10" s="2">
@@ -954,7 +954,7 @@
         <v>292.83365417791754</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2614.4667928000008</v>
       </c>
       <c r="P10" s="2">
@@ -970,11 +970,11 @@
         <v>-73.643462999999997</v>
       </c>
       <c r="C11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.2039587707378662</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="2"/>
-        <v>0.2039587707378662</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="0"/>
         <v>22.847515346812283</v>
       </c>
       <c r="E11" s="2">
@@ -1000,7 +1000,7 @@
         <v>292.57859152230742</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2617.7997323759232</v>
       </c>
       <c r="P11" s="2">
@@ -2450,40 +2450,40 @@
       <c r="L47" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M47" s="7" t="s">
+      <c r="M47" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7"/>
-      <c r="P47" s="7"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
     </row>
     <row r="48" spans="1:16" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L48" s="6"/>
-      <c r="M48" s="7" t="s">
+      <c r="M48" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="7"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
     </row>
     <row r="49" spans="12:16" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M49" s="7" t="s">
+      <c r="M49" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="7"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
     </row>
     <row r="50" spans="12:16" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M50" s="7" t="s">
+      <c r="M50" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>